<commit_message>
beautify RX for screenshot
</commit_message>
<xml_diff>
--- a/Phase2-Transmitter/Frequecy Chart.xlsx
+++ b/Phase2-Transmitter/Frequecy Chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcyle\Desktop\1UoA\2024\ELECT310\ee310-team16\Phase2-Transmitter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{85E06934-97B8-4E0E-8620-0E1A69D35F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A47D26D9-B52E-4F37-B749-44F413B84C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{2470E5AA-A06C-4BB8-A4B0-7097E7434049}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="13">
   <si>
     <t>68k</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>150pF</t>
+  </si>
+  <si>
+    <t>220pF</t>
   </si>
 </sst>
 </file>
@@ -187,17 +190,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4112,19 +4114,19 @@
   <dimension ref="A4:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+      <selection activeCell="Q54" sqref="Q54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4135,13 +4137,13 @@
       <c r="B5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>0</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>65</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>72</v>
       </c>
     </row>
@@ -4152,13 +4154,13 @@
       <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>0.2</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>120</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>44</v>
       </c>
     </row>
@@ -4169,57 +4171,57 @@
       <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>0.4</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>175</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>0.6</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>231</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>0.8</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>286</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>1</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>341</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4230,13 +4232,13 @@
       <c r="B20" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>0</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20">
         <v>65</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="7">
         <v>34</v>
       </c>
     </row>
@@ -4247,13 +4249,13 @@
       <c r="B21" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>0.2</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21">
         <v>120</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="7">
         <v>26</v>
       </c>
     </row>
@@ -4264,24 +4266,24 @@
       <c r="B22" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>0.4</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22">
         <v>175</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="7">
         <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>0.6</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23">
         <v>231</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="7">
         <v>18</v>
       </c>
     </row>
@@ -4292,35 +4294,35 @@
       <c r="B24" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>0.8</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24">
         <v>286</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="7">
         <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="7">
+      <c r="C25" s="6">
         <v>1</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>341</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="8">
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4331,13 +4333,13 @@
       <c r="B35" t="s">
         <v>0</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="5">
         <v>0</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35">
         <v>65</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="7">
         <v>26</v>
       </c>
     </row>
@@ -4348,13 +4350,13 @@
       <c r="B36" t="s">
         <v>1</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="5">
         <v>0.2</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36">
         <v>120</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E36" s="7">
         <v>22</v>
       </c>
     </row>
@@ -4365,24 +4367,24 @@
       <c r="B37" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="5">
         <v>0.4</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37">
         <v>175</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="7">
         <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C38" s="6">
+      <c r="C38" s="5">
         <v>0.6</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38">
         <v>231</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="7">
         <v>16</v>
       </c>
     </row>
@@ -4393,35 +4395,35 @@
       <c r="B39" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="5">
         <v>0.8</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39">
         <v>286</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="7">
         <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C40" s="7">
+      <c r="C40" s="6">
         <v>1</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="1">
         <v>341</v>
       </c>
-      <c r="E40" s="9">
+      <c r="E40" s="8">
         <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E49" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -4432,13 +4434,13 @@
       <c r="B50" t="s">
         <v>0</v>
       </c>
-      <c r="C50" s="6">
+      <c r="C50" s="5">
         <v>0</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50">
         <v>65</v>
       </c>
-      <c r="E50" s="8">
+      <c r="E50" s="7">
         <v>20</v>
       </c>
     </row>
@@ -4449,13 +4451,13 @@
       <c r="B51" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="6">
+      <c r="C51" s="5">
         <v>0.2</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D51">
         <v>120</v>
       </c>
-      <c r="E51" s="8">
+      <c r="E51" s="7">
         <v>18</v>
       </c>
     </row>
@@ -4466,24 +4468,24 @@
       <c r="B52" t="s">
         <v>2</v>
       </c>
-      <c r="C52" s="6">
+      <c r="C52" s="5">
         <v>0.4</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D52">
         <v>175</v>
       </c>
-      <c r="E52" s="8">
+      <c r="E52" s="7">
         <v>16</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C53" s="6">
+      <c r="C53" s="5">
         <v>0.6</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D53">
         <v>231</v>
       </c>
-      <c r="E53" s="8">
+      <c r="E53" s="7">
         <v>14</v>
       </c>
     </row>
@@ -4492,26 +4494,26 @@
         <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>11</v>
-      </c>
-      <c r="C54" s="6">
+        <v>12</v>
+      </c>
+      <c r="C54" s="5">
         <v>0.8</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D54">
         <v>286</v>
       </c>
-      <c r="E54" s="8">
+      <c r="E54" s="7">
         <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="7">
+      <c r="C55" s="6">
         <v>1</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55" s="1">
         <v>341</v>
       </c>
-      <c r="E55" s="9">
+      <c r="E55" s="8">
         <v>11</v>
       </c>
     </row>

</xml_diff>